<commit_message>
Conclusão CTs 2 e 3 usando GET para achar o produto pelo id e pelo nome
</commit_message>
<xml_diff>
--- a/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
+++ b/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Testes - QA\Exercicios treino\API\Serverest\Produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4028AC56-B840-4F43-8A4B-482F8EEED1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D853F31-36F1-430F-9F6E-6BFC5DFC38DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMAÇÕES GERAIS" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -53,17 +53,37 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="3">
     <bk>
       <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Objetivo do Teste</t>
   </si>
@@ -166,6 +186,46 @@
   </si>
   <si>
     <t>Obter base URL e o endpoint</t>
+  </si>
+  <si>
+    <t>Verificar retorno do produto procurado pelo seu id</t>
+  </si>
+  <si>
+    <t>/produtos?_id=0Zao5eWUyyIo14HA</t>
+  </si>
+  <si>
+    <t>Obter a base URL e o código do produto</t>
+  </si>
+  <si>
+    <t>Status 200 OK
+Corpo da resposta deve conter o retorno do produto pesquisado, com as informações dos campos "nome", "preco", "descricao", "quantidade" e "id"</t>
+  </si>
+  <si>
+    <t>Corpo da resposta retornado com seu nome, preco, descrição, quantidade e id</t>
+  </si>
+  <si>
+    <t>Verificar retorno do produto procurado pelo seu nome</t>
+  </si>
+  <si>
+    <t>Obter a base URL e o nome do produto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id = 0Zao5eWUyyIo14HA</t>
+  </si>
+  <si>
+    <t>nome = Generic Wooden Fish</t>
+  </si>
+  <si>
+    <t>/produtos?_id=</t>
+  </si>
+  <si>
+    <t>/produtos?nome=</t>
+  </si>
+  <si>
+    <t>Lista o produto cadastrado pelo seu id</t>
+  </si>
+  <si>
+    <t>Lista o produto cadastrado pelo seu nome</t>
   </si>
 </sst>
 </file>
@@ -304,17 +364,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -374,9 +434,17 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <rv s="0">
     <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -394,6 +462,8 @@
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -716,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2804C6-EE72-47E5-90DC-52B190FC797A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B14" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
@@ -731,7 +801,7 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -740,16 +810,16 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -757,7 +827,7 @@
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -765,13 +835,13 @@
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -779,7 +849,7 @@
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>45752</v>
       </c>
     </row>
@@ -787,7 +857,7 @@
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -804,7 +874,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -838,9 +908,26 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -851,11 +938,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABF6A07-9EA8-4391-AAA5-55F8DE1DFD01}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -941,17 +1028,70 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K3" xr:uid="{8ABF6A07-9EA8-4391-AAA5-55F8DE1DFD01}"/>

</xml_diff>

<commit_message>
Atualização campo 'Autenticação' do doc
</commit_message>
<xml_diff>
--- a/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
+++ b/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Testes - QA\Exercicios treino\API\Serverest\Produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0923CB-6050-4BFB-B87A-C328D9B3D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BF715F-836E-4F16-85E7-5802D89107DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMAÇÕES GERAIS" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Objetivo do Teste</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Lista o produto cadastrado pelo seu nome</t>
+  </si>
+  <si>
+    <t>No Auth</t>
   </si>
 </sst>
 </file>
@@ -786,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2804C6-EE72-47E5-90DC-52B190FC797A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B13:B14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -835,7 +838,9 @@
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -940,9 +945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABF6A07-9EA8-4391-AAA5-55F8DE1DFD01}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2:K4"/>
+    <sheetView showGridLines="0" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Correção do documento Produtos - GET
</commit_message>
<xml_diff>
--- a/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
+++ b/Produtos/Doc de Testes - Serverest - Produtos - GET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Testes - QA\Exercicios treino\API\Serverest\Produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BF715F-836E-4F16-85E7-5802D89107DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D4556D-F7BC-490E-92FA-593AC5AAA380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B8034183-D5CC-4179-9703-4B514E845DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMAÇÕES GERAIS" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2804C6-EE72-47E5-90DC-52B190FC797A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D53ECA8-7E9F-489D-A86E-293B789E29D0}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>